<commit_message>
updated language for the paper section
</commit_message>
<xml_diff>
--- a/public/files/BulkPaperDataUploadSample.xlsx
+++ b/public/files/BulkPaperDataUploadSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\keygentemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\keygenui281224\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{618DBC10-5B94-4430-B16A-C8CDBB862449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E935EE4D-BAB2-4BFE-A0A9-CC5229CCA821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4EC8CBB4-7029-49BC-9CE8-752ADF8378EF}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{4EC8CBB4-7029-49BC-9CE8-752ADF8378EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>S.No.</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Paper Name</t>
+  </si>
+  <si>
+    <t>Paper Language</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2239D9-83E7-42B5-9F82-E9F9956CCB12}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,9 +586,10 @@
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="28.140625" customWidth="1"/>
     <col min="6" max="6" width="49.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,6 +608,9 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">

</xml_diff>

<commit_message>
Fixed search in All generated keys,  question number in type mode in master key
</commit_message>
<xml_diff>
--- a/public/files/BulkPaperDataUploadSample.xlsx
+++ b/public/files/BulkPaperDataUploadSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\keygenui281224\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.24\e\hosted apps\KEYGEN\UI\build\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A10B10-57AF-46AD-BDFD-965B7AA87631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CA3BA9-DC05-4F67-8D63-322856E5EDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Catch No.</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Number of Questions</t>
+  </si>
+  <si>
+    <t>Paper Name</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,8 +88,14 @@
         <fgColor rgb="FFC1E5F5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,11 +118,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,6 +147,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,10 +456,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +474,7 @@
     <col min="8" max="8" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -463,13 +490,16 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>